<commit_message>
added emx for inheritance table
</commit_message>
<xml_diff>
--- a/model/alissa/alissa.xlsx
+++ b/model/alissa/alissa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/molgenis-cosas/model/alissa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8AC591-926E-1C49-AC35-A57F8929B22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B02AE97-5BF4-C540-B375-4C27EEBE0BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{EEB8F3A8-2F0F-3F4D-B4C3-D1DA88451070}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -304,9 +304,6 @@
     <t>alissa_variantexports</t>
   </si>
   <si>
-    <t>identifer: umcgNr + start + transcript + ref</t>
-  </si>
-  <si>
     <t>aggregateable</t>
   </si>
   <si>
@@ -389,6 +386,33 @@
   </si>
   <si>
     <t>variants</t>
+  </si>
+  <si>
+    <t>assignedOn</t>
+  </si>
+  <si>
+    <t>assignedTo</t>
+  </si>
+  <si>
+    <t>thirdParty</t>
+  </si>
+  <si>
+    <t>labResults</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>maternalPatientId</t>
+  </si>
+  <si>
+    <t>paternalPatientId</t>
+  </si>
+  <si>
+    <t>maternalAffectedStatus</t>
+  </si>
+  <si>
+    <t>paternalAffectedStatus</t>
   </si>
 </sst>
 </file>
@@ -784,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56640647-E723-D345-9F08-F2A35A4248EA}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -818,7 +842,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -840,13 +864,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -854,13 +878,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
         <v>109</v>
-      </c>
-      <c r="C5" t="s">
-        <v>110</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -873,11 +897,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A23332-D982-274A-8C02-C7A22BA6D9A9}">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +932,7 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -923,7 +947,7 @@
         <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -1009,13 +1033,13 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1023,13 +1047,13 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1037,10 +1061,10 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
         <v>87</v>
@@ -1133,7 +1157,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>86</v>
@@ -1153,7 +1177,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1164,10 +1188,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
         <v>31</v>
@@ -1175,10 +1199,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
@@ -1186,7 +1210,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
@@ -1197,10 +1221,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -1208,7 +1232,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -1219,10 +1243,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
@@ -1230,7 +1254,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -1241,10 +1265,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
@@ -1252,7 +1276,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
@@ -1263,10 +1287,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>31</v>
@@ -1274,10 +1298,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
@@ -1285,7 +1309,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>53</v>
@@ -1296,10 +1320,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>31</v>
@@ -1307,10 +1331,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
@@ -1318,10 +1342,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
@@ -1329,10 +1353,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
@@ -1340,7 +1364,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
         <v>81</v>
@@ -1351,7 +1375,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
         <v>21</v>
@@ -1365,7 +1389,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
         <v>22</v>
@@ -1379,7 +1403,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
         <v>27</v>
@@ -1396,7 +1420,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
         <v>86</v>
@@ -1411,35 +1435,37 @@
         <v>1</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
         <v>31</v>
-      </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
         <v>31</v>
@@ -1447,27 +1473,21 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>31</v>
-      </c>
-      <c r="F44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
         <v>31</v>
@@ -1475,10 +1495,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
         <v>31</v>
@@ -1486,32 +1506,32 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>31</v>
@@ -1519,10 +1539,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
         <v>31</v>
@@ -1530,10 +1550,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
         <v>31</v>
@@ -1541,10 +1561,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
         <v>31</v>
@@ -1552,10 +1572,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
         <v>31</v>
@@ -1563,10 +1583,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="C54" t="s">
         <v>31</v>
@@ -1574,10 +1594,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="C55" t="s">
         <v>31</v>
@@ -1585,10 +1605,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
         <v>31</v>
@@ -1596,10 +1616,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C57" t="s">
         <v>31</v>
@@ -1607,10 +1627,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
         <v>31</v>
@@ -1618,10 +1638,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
         <v>31</v>
@@ -1629,10 +1649,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
         <v>31</v>
@@ -1640,32 +1660,32 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="C63" t="s">
         <v>31</v>
@@ -1673,404 +1693,750 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>37</v>
+      </c>
+      <c r="I68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>37</v>
+      </c>
+      <c r="I69" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="I70" t="s">
+        <v>81</v>
+      </c>
+      <c r="K70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>87</v>
+      </c>
+      <c r="B72" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" t="b">
+        <v>1</v>
+      </c>
+      <c r="G72" t="b">
+        <v>1</v>
+      </c>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" t="s">
+        <v>42</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>44</v>
+      </c>
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" t="s">
+        <v>45</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
+        <v>48</v>
+      </c>
+      <c r="C82" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" t="s">
+        <v>49</v>
+      </c>
+      <c r="C83" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="C86" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>54</v>
+      </c>
+      <c r="C88" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" t="s">
+        <v>57</v>
+      </c>
+      <c r="C91" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C92" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" t="s">
+        <v>59</v>
+      </c>
+      <c r="C93" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" t="s">
         <v>60</v>
       </c>
-      <c r="C64" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C94" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" t="s">
         <v>61</v>
-      </c>
-      <c r="C65" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>87</v>
-      </c>
-      <c r="B67" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" t="s">
-        <v>66</v>
-      </c>
-      <c r="C70" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" t="s">
-        <v>67</v>
-      </c>
-      <c r="C71" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>87</v>
-      </c>
-      <c r="B72" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>87</v>
-      </c>
-      <c r="B73" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" t="s">
-        <v>70</v>
-      </c>
-      <c r="C74" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>87</v>
-      </c>
-      <c r="B75" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" t="s">
-        <v>73</v>
-      </c>
-      <c r="C77" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" t="s">
-        <v>75</v>
-      </c>
-      <c r="C79" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80" t="s">
-        <v>76</v>
-      </c>
-      <c r="C80" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>87</v>
-      </c>
-      <c r="B81" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>87</v>
-      </c>
-      <c r="B82" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83" t="s">
-        <v>79</v>
-      </c>
-      <c r="C83" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" t="s">
-        <v>80</v>
-      </c>
-      <c r="C84" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>87</v>
-      </c>
-      <c r="B85" t="s">
-        <v>94</v>
-      </c>
-      <c r="C85" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>87</v>
-      </c>
-      <c r="B86" t="s">
-        <v>92</v>
-      </c>
-      <c r="C86" t="s">
-        <v>31</v>
-      </c>
-      <c r="K86" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>87</v>
-      </c>
-      <c r="B87" t="s">
-        <v>93</v>
-      </c>
-      <c r="C87" t="s">
-        <v>31</v>
-      </c>
-      <c r="K87" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>90</v>
-      </c>
-      <c r="C88" t="s">
-        <v>31</v>
-      </c>
-      <c r="K88" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" t="s">
-        <v>21</v>
-      </c>
-      <c r="C90" t="s">
-        <v>37</v>
-      </c>
-      <c r="I90" t="s">
-        <v>81</v>
-      </c>
-      <c r="K90" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>87</v>
-      </c>
-      <c r="B91" t="s">
-        <v>22</v>
-      </c>
-      <c r="C91" t="s">
-        <v>37</v>
-      </c>
-      <c r="I91" t="s">
-        <v>81</v>
-      </c>
-      <c r="K91" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>87</v>
-      </c>
-      <c r="B92" t="s">
-        <v>24</v>
-      </c>
-      <c r="C92" t="s">
-        <v>30</v>
-      </c>
-      <c r="I92" t="s">
-        <v>81</v>
-      </c>
-      <c r="J92" t="b">
-        <v>1</v>
-      </c>
-      <c r="K92" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>87</v>
-      </c>
-      <c r="B93" t="s">
-        <v>25</v>
-      </c>
-      <c r="C93" t="s">
-        <v>31</v>
-      </c>
-      <c r="I93" t="s">
-        <v>81</v>
-      </c>
-      <c r="J93" t="b">
-        <v>1</v>
-      </c>
-      <c r="K93" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>87</v>
-      </c>
-      <c r="B94" t="s">
-        <v>26</v>
-      </c>
-      <c r="C94" t="s">
-        <v>31</v>
-      </c>
-      <c r="I94" t="s">
-        <v>81</v>
-      </c>
-      <c r="K94" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>87</v>
-      </c>
-      <c r="B95" t="s">
-        <v>27</v>
       </c>
       <c r="C95" t="s">
         <v>32</v>
       </c>
-      <c r="I95" t="s">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>87</v>
+      </c>
+      <c r="B98" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>87</v>
+      </c>
+      <c r="B99" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>87</v>
+      </c>
+      <c r="B101" t="s">
+        <v>67</v>
+      </c>
+      <c r="C101" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B102" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>87</v>
+      </c>
+      <c r="B103" t="s">
+        <v>69</v>
+      </c>
+      <c r="C103" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>87</v>
+      </c>
+      <c r="B104" t="s">
+        <v>70</v>
+      </c>
+      <c r="C104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>87</v>
+      </c>
+      <c r="B105" t="s">
+        <v>71</v>
+      </c>
+      <c r="C105" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>87</v>
+      </c>
+      <c r="B106" t="s">
+        <v>72</v>
+      </c>
+      <c r="C106" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107" t="s">
+        <v>73</v>
+      </c>
+      <c r="C107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" t="s">
+        <v>74</v>
+      </c>
+      <c r="C108" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>87</v>
+      </c>
+      <c r="B109" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110" t="s">
+        <v>76</v>
+      </c>
+      <c r="C110" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>87</v>
+      </c>
+      <c r="B111" t="s">
+        <v>77</v>
+      </c>
+      <c r="C111" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>87</v>
+      </c>
+      <c r="B112" t="s">
+        <v>78</v>
+      </c>
+      <c r="C112" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" t="s">
+        <v>79</v>
+      </c>
+      <c r="C113" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>87</v>
+      </c>
+      <c r="B114" t="s">
+        <v>80</v>
+      </c>
+      <c r="C114" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>87</v>
+      </c>
+      <c r="B115" t="s">
+        <v>93</v>
+      </c>
+      <c r="C115" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>87</v>
+      </c>
+      <c r="B116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C116" t="s">
+        <v>31</v>
+      </c>
+      <c r="K116" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>87</v>
+      </c>
+      <c r="B117" t="s">
+        <v>92</v>
+      </c>
+      <c r="C117" t="s">
+        <v>31</v>
+      </c>
+      <c r="K117" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>87</v>
+      </c>
+      <c r="B118" t="s">
+        <v>89</v>
+      </c>
+      <c r="C118" t="s">
+        <v>31</v>
+      </c>
+      <c r="K118" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
         <v>81</v>
       </c>
-      <c r="K95" t="s">
+      <c r="C119" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>87</v>
+      </c>
+      <c r="B120" t="s">
+        <v>21</v>
+      </c>
+      <c r="C120" t="s">
+        <v>37</v>
+      </c>
+      <c r="I120" t="s">
+        <v>81</v>
+      </c>
+      <c r="K120" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>87</v>
+      </c>
+      <c r="B121" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" t="s">
+        <v>37</v>
+      </c>
+      <c r="I121" t="s">
+        <v>81</v>
+      </c>
+      <c r="K121" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>87</v>
+      </c>
+      <c r="B122" t="s">
+        <v>24</v>
+      </c>
+      <c r="C122" t="s">
+        <v>30</v>
+      </c>
+      <c r="I122" t="s">
+        <v>81</v>
+      </c>
+      <c r="J122" t="b">
+        <v>1</v>
+      </c>
+      <c r="K122" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>87</v>
+      </c>
+      <c r="B123" t="s">
+        <v>25</v>
+      </c>
+      <c r="C123" t="s">
+        <v>31</v>
+      </c>
+      <c r="I123" t="s">
+        <v>81</v>
+      </c>
+      <c r="J123" t="b">
+        <v>1</v>
+      </c>
+      <c r="K123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>87</v>
+      </c>
+      <c r="B124" t="s">
+        <v>26</v>
+      </c>
+      <c r="C124" t="s">
+        <v>31</v>
+      </c>
+      <c r="I124" t="s">
+        <v>81</v>
+      </c>
+      <c r="K124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>87</v>
+      </c>
+      <c r="B125" t="s">
+        <v>27</v>
+      </c>
+      <c r="C125" t="s">
+        <v>32</v>
+      </c>
+      <c r="I125" t="s">
+        <v>81</v>
+      </c>
+      <c r="K125" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checked attr to text
</commit_message>
<xml_diff>
--- a/model/alissa/alissa.xlsx
+++ b/model/alissa/alissa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/molgenis-cosas/model/alissa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B02AE97-5BF4-C540-B375-4C27EEBE0BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063B03AE-8363-A847-8A03-D55C01132F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{EEB8F3A8-2F0F-3F4D-B4C3-D1DA88451070}"/>
   </bookViews>
@@ -900,8 +900,8 @@
   <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2144,7 +2144,7 @@
         <v>69</v>
       </c>
       <c r="C103" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finialised alissa mapping scripts
</commit_message>
<xml_diff>
--- a/model/alissa/alissa.xlsx
+++ b/model/alissa/alissa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/molgenis-cosas/model/alissa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063B03AE-8363-A847-8A03-D55C01132F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C016CC-F866-764B-9F8F-1E9358DDD6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{EEB8F3A8-2F0F-3F4D-B4C3-D1DA88451070}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>paternalAffectedStatus</t>
+  </si>
+  <si>
+    <t>inheritanceAlleles</t>
   </si>
 </sst>
 </file>
@@ -897,11 +900,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A23332-D982-274A-8C02-C7A22BA6D9A9}">
-  <dimension ref="A1:K125"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,10 +2276,10 @@
         <v>87</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C115" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
@@ -2284,13 +2287,10 @@
         <v>87</v>
       </c>
       <c r="B116" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C116" t="s">
         <v>31</v>
-      </c>
-      <c r="K116" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -2298,13 +2298,13 @@
         <v>87</v>
       </c>
       <c r="B117" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C117" t="s">
         <v>31</v>
       </c>
       <c r="K117" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
@@ -2312,13 +2312,13 @@
         <v>87</v>
       </c>
       <c r="B118" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C118" t="s">
         <v>31</v>
       </c>
       <c r="K118" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
@@ -2326,10 +2326,13 @@
         <v>87</v>
       </c>
       <c r="B119" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C119" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="K119" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
@@ -2337,16 +2340,10 @@
         <v>87</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="C120" t="s">
-        <v>37</v>
-      </c>
-      <c r="I120" t="s">
-        <v>81</v>
-      </c>
-      <c r="K120" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
@@ -2354,7 +2351,7 @@
         <v>87</v>
       </c>
       <c r="B121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C121" t="s">
         <v>37</v>
@@ -2363,7 +2360,7 @@
         <v>81</v>
       </c>
       <c r="K121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
@@ -2371,19 +2368,16 @@
         <v>87</v>
       </c>
       <c r="B122" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="I122" t="s">
         <v>81</v>
       </c>
-      <c r="J122" t="b">
-        <v>1</v>
-      </c>
       <c r="K122" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
@@ -2391,10 +2385,10 @@
         <v>87</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C123" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I123" t="s">
         <v>81</v>
@@ -2403,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
@@ -2411,7 +2405,7 @@
         <v>87</v>
       </c>
       <c r="B124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C124" t="s">
         <v>31</v>
@@ -2419,8 +2413,11 @@
       <c r="I124" t="s">
         <v>81</v>
       </c>
+      <c r="J124" t="b">
+        <v>1</v>
+      </c>
       <c r="K124" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
@@ -2428,15 +2425,32 @@
         <v>87</v>
       </c>
       <c r="B125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I125" t="s">
         <v>81</v>
       </c>
       <c r="K125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>87</v>
+      </c>
+      <c r="B126" t="s">
+        <v>27</v>
+      </c>
+      <c r="C126" t="s">
+        <v>32</v>
+      </c>
+      <c r="I126" t="s">
+        <v>81</v>
+      </c>
+      <c r="K126" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>